<commit_message>
Updated kernel module data dictionary with recent DB changes
</commit_message>
<xml_diff>
--- a/design/data_model/mosip_kernel_dd.xlsx
+++ b/design/data_model/mosip_kernel_dd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Backup\NasirKhan\MindTree\Digital\Projects\MOSIP\Data Model\DataDictionary\Latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045015\git\commons\design\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E5A214F8-84E8-455A-BB0D-EC19DD7F22BC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9D239DDE-AA7C-498B-897E-3E2D00272E74}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="163">
   <si>
     <t>app_id</t>
   </si>
@@ -477,6 +477,45 @@
   </si>
   <si>
     <t>UIN: Stores pre-generated UINs that are assigned to an individual as part of registration process.</t>
+  </si>
+  <si>
+    <t>prid</t>
+  </si>
+  <si>
+    <t>PRID: Stores pre-generated PRIDs that are assigned to an individual as part of mosip preregistration process</t>
+  </si>
+  <si>
+    <t>vid</t>
+  </si>
+  <si>
+    <t>VID: Stores pre-generated VIDs that are assigned to an individual as part of mosip process.</t>
+  </si>
+  <si>
+    <t>pk_prid_id</t>
+  </si>
+  <si>
+    <t>PRID: Pre-generated PRIDs (Pre registration IDs), which will be used to assign to an individual</t>
+  </si>
+  <si>
+    <t>prid_status</t>
+  </si>
+  <si>
+    <t>PRID Status: Status of the pre-generated PRID, whether it is available, expired or assigned.</t>
+  </si>
+  <si>
+    <t>pk_vid_id</t>
+  </si>
+  <si>
+    <t>VID: Pre-generated VIDs (Vertual Identification Number), which will be used to assign to an individual</t>
+  </si>
+  <si>
+    <t>Expiry Date and Time: Expiry Date and Time of the Vertual ID</t>
+  </si>
+  <si>
+    <t>vid_status</t>
+  </si>
+  <si>
+    <t>VID: Status of the pre-generated VID, whether it is available, expired or assigned.</t>
   </si>
 </sst>
 </file>
@@ -883,33 +922,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C81F4C1-F467-49C6-A81F-F54D1B2B3B09}">
-  <dimension ref="B1:J124"/>
+  <dimension ref="B1:J143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
       <c r="E1" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
@@ -938,7 +977,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -955,7 +994,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
@@ -984,7 +1023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
@@ -1009,7 +1048,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1034,7 +1073,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
@@ -1057,7 +1096,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
@@ -1080,7 +1119,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1144,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1130,7 +1169,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
@@ -1153,7 +1192,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1178,7 +1217,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
@@ -1201,7 +1240,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1263,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1286,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1311,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>49</v>
       </c>
@@ -1289,7 +1328,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>49</v>
       </c>
@@ -1318,7 +1357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
@@ -1341,7 +1380,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>49</v>
       </c>
@@ -1364,7 +1403,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>49</v>
       </c>
@@ -1389,7 +1428,7 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>49</v>
       </c>
@@ -1412,7 +1451,7 @@
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
@@ -1437,7 +1476,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="7" t="s">
         <v>49</v>
       </c>
@@ -1460,7 +1499,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1483,7 +1522,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="7" t="s">
         <v>49</v>
       </c>
@@ -1506,7 +1545,7 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>57</v>
       </c>
@@ -1523,7 +1562,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>57</v>
       </c>
@@ -1552,7 +1591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>57</v>
       </c>
@@ -1579,7 +1618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>57</v>
       </c>
@@ -1602,7 +1641,7 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>57</v>
       </c>
@@ -1625,7 +1664,7 @@
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
@@ -1650,7 +1689,7 @@
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="7" t="s">
         <v>57</v>
       </c>
@@ -1673,7 +1712,7 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>57</v>
       </c>
@@ -1698,7 +1737,7 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="7" t="s">
         <v>57</v>
       </c>
@@ -1721,7 +1760,7 @@
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="7" t="s">
         <v>57</v>
       </c>
@@ -1744,7 +1783,7 @@
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="7" t="s">
         <v>57</v>
       </c>
@@ -1767,7 +1806,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>61</v>
       </c>
@@ -1784,7 +1823,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>61</v>
       </c>
@@ -1813,7 +1852,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
         <v>61</v>
       </c>
@@ -1838,7 +1877,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="7" t="s">
         <v>61</v>
       </c>
@@ -1861,7 +1900,7 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="7" t="s">
         <v>61</v>
       </c>
@@ -1884,7 +1923,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="7" t="s">
         <v>61</v>
       </c>
@@ -1909,7 +1948,7 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="7" t="s">
         <v>61</v>
       </c>
@@ -1932,7 +1971,7 @@
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="7" t="s">
         <v>61</v>
       </c>
@@ -1957,7 +1996,7 @@
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="7" t="s">
         <v>61</v>
       </c>
@@ -1980,7 +2019,7 @@
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
         <v>61</v>
       </c>
@@ -2003,7 +2042,7 @@
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="7" t="s">
         <v>61</v>
       </c>
@@ -2026,7 +2065,7 @@
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="5" t="s">
         <v>71</v>
       </c>
@@ -2043,7 +2082,7 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" s="7" t="s">
         <v>71</v>
       </c>
@@ -2072,7 +2111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="7" t="s">
         <v>71</v>
       </c>
@@ -2097,7 +2136,7 @@
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="7" t="s">
         <v>71</v>
       </c>
@@ -2122,7 +2161,7 @@
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" s="7" t="s">
         <v>71</v>
       </c>
@@ -2147,7 +2186,7 @@
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="7" t="s">
         <v>71</v>
       </c>
@@ -2170,7 +2209,7 @@
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" s="7" t="s">
         <v>71</v>
       </c>
@@ -2193,7 +2232,7 @@
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="7" t="s">
         <v>71</v>
       </c>
@@ -2216,7 +2255,7 @@
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="7" t="s">
         <v>71</v>
       </c>
@@ -2241,7 +2280,7 @@
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" s="7" t="s">
         <v>71</v>
       </c>
@@ -2266,7 +2305,7 @@
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
         <v>71</v>
       </c>
@@ -2291,7 +2330,7 @@
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" s="7" t="s">
         <v>71</v>
       </c>
@@ -2314,7 +2353,7 @@
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="7" t="s">
         <v>71</v>
       </c>
@@ -2339,7 +2378,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" s="7" t="s">
         <v>71</v>
       </c>
@@ -2362,7 +2401,7 @@
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="7" t="s">
         <v>71</v>
       </c>
@@ -2385,7 +2424,7 @@
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="7" t="s">
         <v>71</v>
       </c>
@@ -2408,7 +2447,7 @@
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" s="5" t="s">
         <v>85</v>
       </c>
@@ -2425,7 +2464,7 @@
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="7" t="s">
         <v>85</v>
       </c>
@@ -2454,7 +2493,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="7" t="s">
         <v>85</v>
       </c>
@@ -2483,7 +2522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="7" t="s">
         <v>85</v>
       </c>
@@ -2508,7 +2547,7 @@
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="7" t="s">
         <v>85</v>
       </c>
@@ -2533,7 +2572,7 @@
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="7" t="s">
         <v>85</v>
       </c>
@@ -2562,7 +2601,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B71" s="7" t="s">
         <v>85</v>
       </c>
@@ -2585,7 +2624,7 @@
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B72" s="7" t="s">
         <v>85</v>
       </c>
@@ -2610,7 +2649,7 @@
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B73" s="7" t="s">
         <v>85</v>
       </c>
@@ -2633,7 +2672,7 @@
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="7" t="s">
         <v>85</v>
       </c>
@@ -2658,7 +2697,7 @@
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="7" t="s">
         <v>85</v>
       </c>
@@ -2681,7 +2720,7 @@
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B76" s="7" t="s">
         <v>85</v>
       </c>
@@ -2706,7 +2745,7 @@
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" s="7" t="s">
         <v>85</v>
       </c>
@@ -2729,7 +2768,7 @@
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B78" s="7" t="s">
         <v>85</v>
       </c>
@@ -2752,7 +2791,7 @@
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B79" s="7" t="s">
         <v>85</v>
       </c>
@@ -2775,7 +2814,7 @@
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B80" s="5" t="s">
         <v>101</v>
       </c>
@@ -2792,7 +2831,7 @@
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B81" s="7" t="s">
         <v>101</v>
       </c>
@@ -2821,7 +2860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B82" s="7" t="s">
         <v>101</v>
       </c>
@@ -2846,7 +2885,7 @@
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B83" s="7" t="s">
         <v>101</v>
       </c>
@@ -2871,7 +2910,7 @@
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B84" s="7" t="s">
         <v>101</v>
       </c>
@@ -2896,7 +2935,7 @@
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B85" s="7" t="s">
         <v>101</v>
       </c>
@@ -2921,7 +2960,7 @@
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B86" s="7" t="s">
         <v>101</v>
       </c>
@@ -2946,7 +2985,7 @@
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
     </row>
-    <row r="87" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B87" s="7" t="s">
         <v>101</v>
       </c>
@@ -2971,7 +3010,7 @@
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B88" s="7" t="s">
         <v>101</v>
       </c>
@@ -2994,7 +3033,7 @@
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B89" s="7" t="s">
         <v>101</v>
       </c>
@@ -3019,7 +3058,7 @@
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
     </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B90" s="7" t="s">
         <v>101</v>
       </c>
@@ -3042,7 +3081,7 @@
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
     </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B91" s="7" t="s">
         <v>101</v>
       </c>
@@ -3067,7 +3106,7 @@
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B92" s="7" t="s">
         <v>101</v>
       </c>
@@ -3090,7 +3129,7 @@
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B93" s="7" t="s">
         <v>101</v>
       </c>
@@ -3113,7 +3152,7 @@
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B94" s="7" t="s">
         <v>101</v>
       </c>
@@ -3136,7 +3175,7 @@
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B95" s="5" t="s">
         <v>114</v>
       </c>
@@ -3153,7 +3192,7 @@
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B96" s="7" t="s">
         <v>114</v>
       </c>
@@ -3182,7 +3221,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" s="7" t="s">
         <v>114</v>
       </c>
@@ -3211,7 +3250,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98" s="7" t="s">
         <v>114</v>
       </c>
@@ -3234,7 +3273,7 @@
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" s="7" t="s">
         <v>114</v>
       </c>
@@ -3259,7 +3298,7 @@
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" s="7" t="s">
         <v>114</v>
       </c>
@@ -3284,7 +3323,7 @@
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B101" s="7" t="s">
         <v>114</v>
       </c>
@@ -3309,7 +3348,7 @@
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" s="7" t="s">
         <v>114</v>
       </c>
@@ -3334,7 +3373,7 @@
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B103" s="7" t="s">
         <v>114</v>
       </c>
@@ -3359,7 +3398,7 @@
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B104" s="7" t="s">
         <v>114</v>
       </c>
@@ -3384,7 +3423,7 @@
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B105" s="7" t="s">
         <v>114</v>
       </c>
@@ -3409,7 +3448,7 @@
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B106" s="7" t="s">
         <v>114</v>
       </c>
@@ -3434,7 +3473,7 @@
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B107" s="7" t="s">
         <v>114</v>
       </c>
@@ -3459,7 +3498,7 @@
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B108" s="7" t="s">
         <v>114</v>
       </c>
@@ -3484,7 +3523,7 @@
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B109" s="7" t="s">
         <v>114</v>
       </c>
@@ -3509,7 +3548,7 @@
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B110" s="7" t="s">
         <v>114</v>
       </c>
@@ -3534,7 +3573,7 @@
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B111" s="7" t="s">
         <v>114</v>
       </c>
@@ -3557,7 +3596,7 @@
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B112" s="7" t="s">
         <v>114</v>
       </c>
@@ -3582,7 +3621,7 @@
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B113" s="7" t="s">
         <v>114</v>
       </c>
@@ -3605,7 +3644,7 @@
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B114" s="7" t="s">
         <v>114</v>
       </c>
@@ -3628,7 +3667,7 @@
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B115" s="7" t="s">
         <v>114</v>
       </c>
@@ -3651,7 +3690,7 @@
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B116" s="5" t="s">
         <v>136</v>
       </c>
@@ -3668,7 +3707,7 @@
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B117" s="7" t="s">
         <v>136</v>
       </c>
@@ -3697,7 +3736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B118" s="7" t="s">
         <v>136</v>
       </c>
@@ -3722,7 +3761,7 @@
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B119" s="7" t="s">
         <v>136</v>
       </c>
@@ -3747,7 +3786,7 @@
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B120" s="7" t="s">
         <v>136</v>
       </c>
@@ -3770,7 +3809,7 @@
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B121" s="7" t="s">
         <v>136</v>
       </c>
@@ -3795,7 +3834,7 @@
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B122" s="7" t="s">
         <v>136</v>
       </c>
@@ -3818,7 +3857,7 @@
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B123" s="7" t="s">
         <v>136</v>
       </c>
@@ -3841,7 +3880,7 @@
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B124" s="7" t="s">
         <v>136</v>
       </c>
@@ -3863,6 +3902,451 @@
       </c>
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B125" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B126" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E126" s="7">
+        <v>1</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G126" s="7">
+        <v>36</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I126" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="J126" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B127" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E127" s="7">
+        <v>2</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G127" s="7">
+        <v>16</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+    </row>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B128" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E128" s="7">
+        <v>3</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G128" s="7">
+        <v>256</v>
+      </c>
+      <c r="H128" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I128" s="7"/>
+      <c r="J128" s="7"/>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B129" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E129" s="7">
+        <v>4</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G129" s="7"/>
+      <c r="H129" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I129" s="7"/>
+      <c r="J129" s="7"/>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B130" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E130" s="7">
+        <v>5</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G130" s="7">
+        <v>256</v>
+      </c>
+      <c r="H130" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" s="7"/>
+      <c r="J130" s="7"/>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B131" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E131" s="7">
+        <v>6</v>
+      </c>
+      <c r="F131" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G131" s="7"/>
+      <c r="H131" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I131" s="7"/>
+      <c r="J131" s="7"/>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B132" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E132" s="7">
+        <v>7</v>
+      </c>
+      <c r="F132" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G132" s="7"/>
+      <c r="H132" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="7"/>
+      <c r="J132" s="7"/>
+    </row>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B133" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E133" s="7">
+        <v>8</v>
+      </c>
+      <c r="F133" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G133" s="7"/>
+      <c r="H133" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+    </row>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B134" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="5"/>
+      <c r="G134" s="5"/>
+      <c r="H134" s="5"/>
+      <c r="I134" s="5"/>
+      <c r="J134" s="5"/>
+    </row>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B135" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E135" s="7">
+        <v>1</v>
+      </c>
+      <c r="F135" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G135" s="7">
+        <v>36</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I135" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B136" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E136" s="7">
+        <v>2</v>
+      </c>
+      <c r="F136" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G136" s="7"/>
+      <c r="H136" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I136" s="7"/>
+      <c r="J136" s="7"/>
+    </row>
+    <row r="137" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B137" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E137" s="7">
+        <v>3</v>
+      </c>
+      <c r="F137" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G137" s="7">
+        <v>16</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B138" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E138" s="7">
+        <v>4</v>
+      </c>
+      <c r="F138" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G138" s="7">
+        <v>256</v>
+      </c>
+      <c r="H138" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I138" s="7"/>
+      <c r="J138" s="7"/>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B139" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E139" s="7">
+        <v>5</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G139" s="7"/>
+      <c r="H139" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I139" s="7"/>
+      <c r="J139" s="7"/>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B140" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E140" s="7">
+        <v>6</v>
+      </c>
+      <c r="F140" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G140" s="7">
+        <v>256</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I140" s="7"/>
+      <c r="J140" s="7"/>
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B141" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D141" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E141" s="7">
+        <v>7</v>
+      </c>
+      <c r="F141" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G141" s="7"/>
+      <c r="H141" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+    </row>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B142" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E142" s="7">
+        <v>8</v>
+      </c>
+      <c r="F142" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G142" s="7"/>
+      <c r="H142" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I142" s="7"/>
+      <c r="J142" s="7"/>
+    </row>
+    <row r="143" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B143" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E143" s="7">
+        <v>9</v>
+      </c>
+      <c r="F143" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G143" s="7"/>
+      <c r="H143" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
     </row>
   </sheetData>
   <sortState ref="B4:J124">
@@ -3870,34 +4354,35 @@
     <sortCondition ref="E1:E1048576"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0627A259-5EE8-48C9-A0A8-B000CB5A99AC}">
-  <dimension ref="B2:L116"/>
+  <dimension ref="B2:L132"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L115"/>
+    <sheetView topLeftCell="D130" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="87.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="87.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3932,7 +4417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -3967,7 +4452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -3998,7 +4483,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
@@ -4029,7 +4514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -4058,7 +4543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -4087,7 +4572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -4118,7 +4603,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -4149,7 +4634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
@@ -4178,7 +4663,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -4209,7 +4694,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
@@ -4238,7 +4723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
@@ -4267,7 +4752,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
@@ -4296,7 +4781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
@@ -4327,7 +4812,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
@@ -4362,7 +4847,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -4391,7 +4876,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
@@ -4420,7 +4905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
@@ -4451,7 +4936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>17</v>
       </c>
@@ -4480,7 +4965,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
@@ -4511,7 +4996,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>17</v>
       </c>
@@ -4540,7 +5025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4569,7 +5054,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4598,7 +5083,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>17</v>
       </c>
@@ -4633,7 +5118,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
@@ -4666,7 +5151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
@@ -4695,7 +5180,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
@@ -4724,7 +5209,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
@@ -4755,7 +5240,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
@@ -4784,7 +5269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
@@ -4815,7 +5300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>17</v>
       </c>
@@ -4844,7 +5329,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>17</v>
       </c>
@@ -4873,7 +5358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>17</v>
       </c>
@@ -4902,7 +5387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>17</v>
       </c>
@@ -4937,7 +5422,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
@@ -4968,7 +5453,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>17</v>
       </c>
@@ -4997,7 +5482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>17</v>
       </c>
@@ -5026,7 +5511,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>17</v>
       </c>
@@ -5057,7 +5542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>17</v>
       </c>
@@ -5086,7 +5571,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>17</v>
       </c>
@@ -5117,7 +5602,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>17</v>
       </c>
@@ -5146,7 +5631,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>17</v>
       </c>
@@ -5175,7 +5660,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>17</v>
       </c>
@@ -5204,7 +5689,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>17</v>
       </c>
@@ -5239,7 +5724,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>17</v>
       </c>
@@ -5270,7 +5755,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>17</v>
       </c>
@@ -5301,7 +5786,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>17</v>
       </c>
@@ -5332,7 +5817,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>17</v>
       </c>
@@ -5361,7 +5846,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>17</v>
       </c>
@@ -5390,7 +5875,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
         <v>17</v>
       </c>
@@ -5419,7 +5904,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
         <v>17</v>
       </c>
@@ -5450,7 +5935,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>17</v>
       </c>
@@ -5481,7 +5966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>17</v>
       </c>
@@ -5512,7 +5997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
         <v>17</v>
       </c>
@@ -5541,7 +6026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B56" s="2" t="s">
         <v>17</v>
       </c>
@@ -5572,7 +6057,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>17</v>
       </c>
@@ -5601,7 +6086,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
         <v>17</v>
       </c>
@@ -5630,7 +6115,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
         <v>17</v>
       </c>
@@ -5659,7 +6144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
         <v>17</v>
       </c>
@@ -5694,7 +6179,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B61" s="2" t="s">
         <v>17</v>
       </c>
@@ -5729,7 +6214,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B62" s="2" t="s">
         <v>17</v>
       </c>
@@ -5760,7 +6245,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
         <v>17</v>
       </c>
@@ -5791,7 +6276,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B64" s="2" t="s">
         <v>17</v>
       </c>
@@ -5826,7 +6311,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B65" s="2" t="s">
         <v>17</v>
       </c>
@@ -5855,7 +6340,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
         <v>17</v>
       </c>
@@ -5886,7 +6371,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>17</v>
       </c>
@@ -5915,7 +6400,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B68" s="2" t="s">
         <v>17</v>
       </c>
@@ -5946,7 +6431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B69" s="2" t="s">
         <v>17</v>
       </c>
@@ -5975,7 +6460,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B70" s="2" t="s">
         <v>17</v>
       </c>
@@ -6006,7 +6491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B71" s="2" t="s">
         <v>17</v>
       </c>
@@ -6035,7 +6520,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
         <v>17</v>
       </c>
@@ -6064,7 +6549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B73" s="2" t="s">
         <v>17</v>
       </c>
@@ -6093,7 +6578,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
         <v>17</v>
       </c>
@@ -6128,7 +6613,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B75" s="2" t="s">
         <v>17</v>
       </c>
@@ -6159,7 +6644,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B76" s="2" t="s">
         <v>17</v>
       </c>
@@ -6190,7 +6675,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B77" s="2" t="s">
         <v>17</v>
       </c>
@@ -6221,7 +6706,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B78" s="2" t="s">
         <v>17</v>
       </c>
@@ -6252,7 +6737,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B79" s="2" t="s">
         <v>17</v>
       </c>
@@ -6283,7 +6768,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B80" s="2" t="s">
         <v>17</v>
       </c>
@@ -6314,7 +6799,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B81" s="2" t="s">
         <v>17</v>
       </c>
@@ -6343,7 +6828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B82" s="2" t="s">
         <v>17</v>
       </c>
@@ -6374,7 +6859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B83" s="2" t="s">
         <v>17</v>
       </c>
@@ -6403,7 +6888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B84" s="2" t="s">
         <v>17</v>
       </c>
@@ -6434,7 +6919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B85" s="2" t="s">
         <v>17</v>
       </c>
@@ -6463,7 +6948,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B86" s="2" t="s">
         <v>17</v>
       </c>
@@ -6492,7 +6977,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B87" s="2" t="s">
         <v>17</v>
       </c>
@@ -6521,7 +7006,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B88" s="2" t="s">
         <v>17</v>
       </c>
@@ -6556,7 +7041,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B89" s="2" t="s">
         <v>17</v>
       </c>
@@ -6591,7 +7076,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B90" s="2" t="s">
         <v>17</v>
       </c>
@@ -6620,7 +7105,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B91" s="2" t="s">
         <v>17</v>
       </c>
@@ -6651,7 +7136,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B92" s="2" t="s">
         <v>17</v>
       </c>
@@ -6682,7 +7167,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B93" s="2" t="s">
         <v>17</v>
       </c>
@@ -6713,7 +7198,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B94" s="2" t="s">
         <v>17</v>
       </c>
@@ -6744,7 +7229,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B95" s="2" t="s">
         <v>17</v>
       </c>
@@ -6775,7 +7260,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B96" s="2" t="s">
         <v>17</v>
       </c>
@@ -6806,7 +7291,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B97" s="2" t="s">
         <v>17</v>
       </c>
@@ -6837,7 +7322,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B98" s="2" t="s">
         <v>17</v>
       </c>
@@ -6868,7 +7353,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B99" s="2" t="s">
         <v>17</v>
       </c>
@@ -6899,7 +7384,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B100" s="2" t="s">
         <v>17</v>
       </c>
@@ -6930,7 +7415,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B101" s="2" t="s">
         <v>17</v>
       </c>
@@ -6961,7 +7446,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B102" s="2" t="s">
         <v>17</v>
       </c>
@@ -6992,7 +7477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B103" s="2" t="s">
         <v>17</v>
       </c>
@@ -7021,7 +7506,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B104" s="2" t="s">
         <v>17</v>
       </c>
@@ -7052,7 +7537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B105" s="2" t="s">
         <v>17</v>
       </c>
@@ -7081,7 +7566,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B106" s="2" t="s">
         <v>17</v>
       </c>
@@ -7110,7 +7595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B107" s="2" t="s">
         <v>17</v>
       </c>
@@ -7139,7 +7624,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B108" s="2" t="s">
         <v>17</v>
       </c>
@@ -7174,7 +7659,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B109" s="2" t="s">
         <v>17</v>
       </c>
@@ -7205,7 +7690,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B110" s="2" t="s">
         <v>17</v>
       </c>
@@ -7236,7 +7721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B111" s="2" t="s">
         <v>17</v>
       </c>
@@ -7265,7 +7750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B112" s="2" t="s">
         <v>17</v>
       </c>
@@ -7296,7 +7781,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B113" s="2" t="s">
         <v>17</v>
       </c>
@@ -7325,7 +7810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B114" s="2" t="s">
         <v>17</v>
       </c>
@@ -7354,7 +7839,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B115" s="2" t="s">
         <v>17</v>
       </c>
@@ -7383,18 +7868,522 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="2"/>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B116" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F116" s="2">
+        <v>1</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H116" s="2">
+        <v>36</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J116" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K116" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L116" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B117" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F117" s="2">
+        <v>2</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H117" s="2">
+        <v>16</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B118" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F118" s="2">
+        <v>3</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H118" s="2">
+        <v>256</v>
+      </c>
+      <c r="I118" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B119" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F119" s="2">
+        <v>4</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B120" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F120" s="2">
+        <v>5</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H120" s="2">
+        <v>256</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B121" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F121" s="2">
+        <v>6</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B122" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F122" s="2">
+        <v>7</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B123" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F123" s="2">
+        <v>8</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B124" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F124" s="2">
+        <v>1</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H124" s="2">
+        <v>36</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B125" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F125" s="2">
+        <v>2</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B126" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F126" s="2">
+        <v>3</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H126" s="2">
+        <v>16</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B127" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="2">
+        <v>4</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H127" s="2">
+        <v>256</v>
+      </c>
+      <c r="I127" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="L127" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B128" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F128" s="2">
+        <v>5</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B129" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F129" s="2">
+        <v>6</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H129" s="2">
+        <v>256</v>
+      </c>
+      <c r="I129" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+      <c r="L129" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B130" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F130" s="2">
+        <v>7</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+      <c r="L130" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B131" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F131" s="2">
+        <v>8</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B132" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F132" s="2">
+        <v>9</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H132" s="2"/>
+      <c r="I132" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132" s="2"/>
+      <c r="K132" s="2"/>
+      <c r="L132" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7404,21 +8393,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021FEEDB-BD91-4DE8-AEB7-095BE154130D}">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:L11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="118.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -7432,7 +8421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
@@ -7446,7 +8435,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
@@ -7460,7 +8449,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
@@ -7474,7 +8463,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -7488,7 +8477,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -7502,7 +8491,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -7516,7 +8505,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -7530,7 +8519,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
@@ -7544,7 +8533,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -7558,11 +8547,39 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>